<commit_message>
UploadHomework and results of exam 1
</commit_message>
<xml_diff>
--- a/Materials/大数据菁英班成绩单（第一学期）.xlsx
+++ b/Materials/大数据菁英班成绩单（第一学期）.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28000" windowHeight="17540"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28000" windowHeight="17540" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="sum" sheetId="1" r:id="rId1"/>
     <sheet name="class2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="class3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="123">
   <si>
     <t>李婉荣</t>
   </si>
@@ -639,7 +639,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -664,6 +664,9 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -686,15 +689,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1000,75 +994,75 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
-      <selection activeCell="I92" sqref="I92"/>
+    <sheetView topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="F57" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="0" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="8.83203125" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="14"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="15"/>
     </row>
     <row r="2" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="12"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="15"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="16"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
+      <c r="A4" s="9"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
       <c r="D4" s="7">
         <v>42455</v>
       </c>
@@ -1106,7 +1100,7 @@
         <v>1</v>
       </c>
       <c r="F5" s="3" t="b">
-        <f>ISNA(VLOOKUP(B5,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B5,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G5" s="3">
@@ -1136,7 +1130,7 @@
         <v>1</v>
       </c>
       <c r="F6" s="3" t="b">
-        <f>ISNA(VLOOKUP(B6,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B6,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G6" s="3">
@@ -1166,7 +1160,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="3" t="b">
-        <f>ISNA(VLOOKUP(B7,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B7,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G7" s="3">
@@ -1196,7 +1190,7 @@
         <v>1</v>
       </c>
       <c r="F8" s="3" t="b">
-        <f>ISNA(VLOOKUP(B8,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B8,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G8" s="3">
@@ -1226,7 +1220,7 @@
         <v>1</v>
       </c>
       <c r="F9" s="3" t="b">
-        <f>ISNA(VLOOKUP(B9,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B9,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G9" s="3">
@@ -1256,7 +1250,7 @@
         <v>1</v>
       </c>
       <c r="F10" s="3" t="b">
-        <f>ISNA(VLOOKUP(B10,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B10,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G10" s="3">
@@ -1286,7 +1280,7 @@
         <v>1</v>
       </c>
       <c r="F11" s="3" t="b">
-        <f>ISNA(VLOOKUP(B11,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B11,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G11" s="3">
@@ -1316,7 +1310,7 @@
         <v>1</v>
       </c>
       <c r="F12" s="3" t="b">
-        <f>ISNA(VLOOKUP(B12,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B12,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G12" s="3">
@@ -1346,7 +1340,7 @@
         <v>1</v>
       </c>
       <c r="F13" s="3" t="b">
-        <f>ISNA(VLOOKUP(B13,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B13,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G13" s="3">
@@ -1376,7 +1370,7 @@
         <v>1</v>
       </c>
       <c r="F14" s="3" t="b">
-        <f>ISNA(VLOOKUP(B14,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B14,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G14" s="3">
@@ -1405,7 +1399,7 @@
       <c r="E15" s="3">
         <v>1</v>
       </c>
-      <c r="F15" s="16" t="s">
+      <c r="F15" s="8" t="s">
         <v>122</v>
       </c>
       <c r="G15" s="3">
@@ -1434,7 +1428,7 @@
         <v>1</v>
       </c>
       <c r="F16" s="3" t="b">
-        <f>ISNA(VLOOKUP(B16,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B16,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G16" s="3">
@@ -1464,7 +1458,7 @@
         <v>1</v>
       </c>
       <c r="F17" s="3" t="b">
-        <f>ISNA(VLOOKUP(B17,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B17,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G17" s="3">
@@ -1494,7 +1488,7 @@
         <v>1</v>
       </c>
       <c r="F18" s="3" t="b">
-        <f>ISNA(VLOOKUP(B18,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B18,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G18" s="3">
@@ -1524,7 +1518,7 @@
         <v>1</v>
       </c>
       <c r="F19" s="3" t="b">
-        <f>ISNA(VLOOKUP(B19,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B19,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G19" s="3">
@@ -1554,7 +1548,7 @@
         <v>1</v>
       </c>
       <c r="F20" s="3" t="b">
-        <f>ISNA(VLOOKUP(B20,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B20,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G20" s="3">
@@ -1584,7 +1578,7 @@
         <v>1</v>
       </c>
       <c r="F21" s="3" t="b">
-        <f>ISNA(VLOOKUP(B21,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B21,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G21" s="3">
@@ -1614,7 +1608,7 @@
         <v>1</v>
       </c>
       <c r="F22" s="3" t="b">
-        <f>ISNA(VLOOKUP(B22,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B22,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G22" s="3">
@@ -1644,7 +1638,7 @@
         <v>1</v>
       </c>
       <c r="F23" s="3" t="b">
-        <f>ISNA(VLOOKUP(B23,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B23,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G23" s="3">
@@ -1674,7 +1668,7 @@
         <v>1</v>
       </c>
       <c r="F24" s="3" t="b">
-        <f>ISNA(VLOOKUP(B24,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B24,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G24" s="3">
@@ -1704,7 +1698,7 @@
         <v>1</v>
       </c>
       <c r="F25" s="3" t="b">
-        <f>ISNA(VLOOKUP(B25,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B25,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G25" s="3">
@@ -1734,7 +1728,7 @@
         <v>1</v>
       </c>
       <c r="F26" s="3" t="b">
-        <f>ISNA(VLOOKUP(B26,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B26,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G26" s="3">
@@ -1764,7 +1758,7 @@
         <v>1</v>
       </c>
       <c r="F27" s="3" t="b">
-        <f>ISNA(VLOOKUP(B27,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B27,class2!$A$1:$B$86,2,FALSE))</f>
         <v>1</v>
       </c>
       <c r="G27" s="3">
@@ -1794,7 +1788,7 @@
         <v>1</v>
       </c>
       <c r="F28" s="3" t="b">
-        <f>ISNA(VLOOKUP(B28,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B28,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G28" s="3">
@@ -1824,7 +1818,7 @@
         <v>1</v>
       </c>
       <c r="F29" s="3" t="b">
-        <f>ISNA(VLOOKUP(B29,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B29,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G29" s="3">
@@ -1854,7 +1848,7 @@
         <v>1</v>
       </c>
       <c r="F30" s="3" t="b">
-        <f>ISNA(VLOOKUP(B30,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B30,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G30" s="3">
@@ -1884,7 +1878,7 @@
         <v>1</v>
       </c>
       <c r="F31" s="3" t="b">
-        <f>ISNA(VLOOKUP(B31,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B31,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G31" s="3">
@@ -1914,7 +1908,7 @@
         <v>1</v>
       </c>
       <c r="F32" s="3" t="b">
-        <f>ISNA(VLOOKUP(B32,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B32,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G32" s="3">
@@ -1944,7 +1938,7 @@
         <v>1</v>
       </c>
       <c r="F33" s="3" t="b">
-        <f>ISNA(VLOOKUP(B33,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B33,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G33" s="3">
@@ -1974,7 +1968,7 @@
         <v>1</v>
       </c>
       <c r="F34" s="3" t="b">
-        <f>ISNA(VLOOKUP(B34,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B34,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G34" s="3">
@@ -2004,7 +1998,7 @@
         <v>1</v>
       </c>
       <c r="F35" s="3" t="b">
-        <f>ISNA(VLOOKUP(B35,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B35,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G35" s="3">
@@ -2034,7 +2028,7 @@
         <v>1</v>
       </c>
       <c r="F36" s="3" t="b">
-        <f>ISNA(VLOOKUP(B36,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B36,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G36" s="3">
@@ -2064,7 +2058,7 @@
         <v>1</v>
       </c>
       <c r="F37" s="3" t="b">
-        <f>ISNA(VLOOKUP(B37,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B37,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G37" s="3">
@@ -2094,7 +2088,7 @@
         <v>1</v>
       </c>
       <c r="F38" s="3" t="b">
-        <f>ISNA(VLOOKUP(B38,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B38,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G38" s="3">
@@ -2124,7 +2118,7 @@
         <v>1</v>
       </c>
       <c r="F39" s="3" t="b">
-        <f>ISNA(VLOOKUP(B39,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B39,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G39" s="3">
@@ -2154,7 +2148,7 @@
         <v>1</v>
       </c>
       <c r="F40" s="3" t="b">
-        <f>ISNA(VLOOKUP(B40,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B40,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G40" s="3">
@@ -2184,7 +2178,7 @@
         <v>1</v>
       </c>
       <c r="F41" s="3" t="b">
-        <f>ISNA(VLOOKUP(B41,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B41,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G41" s="3">
@@ -2214,7 +2208,7 @@
         <v>1</v>
       </c>
       <c r="F42" s="3" t="b">
-        <f>ISNA(VLOOKUP(B42,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B42,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G42" s="3">
@@ -2244,7 +2238,7 @@
         <v>1</v>
       </c>
       <c r="F43" s="3" t="b">
-        <f>ISNA(VLOOKUP(B43,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B43,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G43" s="3">
@@ -2274,7 +2268,7 @@
         <v>1</v>
       </c>
       <c r="F44" s="3" t="b">
-        <f>ISNA(VLOOKUP(B44,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B44,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G44" s="3">
@@ -2304,7 +2298,7 @@
         <v>1</v>
       </c>
       <c r="F45" s="3" t="b">
-        <f>ISNA(VLOOKUP(B45,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B45,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G45" s="3">
@@ -2334,7 +2328,7 @@
         <v>1</v>
       </c>
       <c r="F46" s="3" t="b">
-        <f>ISNA(VLOOKUP(B46,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B46,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G46" s="3">
@@ -2364,7 +2358,7 @@
         <v>1</v>
       </c>
       <c r="F47" s="3" t="b">
-        <f>ISNA(VLOOKUP(B47,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B47,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G47" s="3">
@@ -2394,7 +2388,7 @@
         <v>1</v>
       </c>
       <c r="F48" s="3" t="b">
-        <f>ISNA(VLOOKUP(B48,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B48,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G48" s="3">
@@ -2424,7 +2418,7 @@
         <v>1</v>
       </c>
       <c r="F49" s="3" t="b">
-        <f>ISNA(VLOOKUP(B49,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B49,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G49" s="3">
@@ -2454,7 +2448,7 @@
         <v>1</v>
       </c>
       <c r="F50" s="3" t="b">
-        <f>ISNA(VLOOKUP(B50,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B50,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G50" s="3">
@@ -2484,7 +2478,7 @@
         <v>1</v>
       </c>
       <c r="F51" s="3" t="b">
-        <f>ISNA(VLOOKUP(B51,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B51,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G51" s="3">
@@ -2514,7 +2508,7 @@
         <v>1</v>
       </c>
       <c r="F52" s="3" t="b">
-        <f>ISNA(VLOOKUP(B52,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B52,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G52" s="3">
@@ -2544,7 +2538,7 @@
         <v>1</v>
       </c>
       <c r="F53" s="3" t="b">
-        <f>ISNA(VLOOKUP(B53,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B53,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G53" s="3">
@@ -2574,7 +2568,7 @@
         <v>1</v>
       </c>
       <c r="F54" s="3" t="b">
-        <f>ISNA(VLOOKUP(B54,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B54,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G54" s="3">
@@ -2604,12 +2598,12 @@
         <v>1</v>
       </c>
       <c r="F55" s="3" t="b">
-        <f>ISNA(VLOOKUP(B55,class2!$A$1:$B$83,2,FALSE))</f>
-        <v>1</v>
+        <f>ISNA(VLOOKUP(B55,class2!$A$1:$B$86,2,FALSE))</f>
+        <v>0</v>
       </c>
       <c r="G55" s="3">
         <f t="shared" si="0"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="H55" s="3"/>
       <c r="I55" s="3"/>
@@ -2634,7 +2628,7 @@
         <v>1</v>
       </c>
       <c r="F56" s="3" t="b">
-        <f>ISNA(VLOOKUP(B56,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B56,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G56" s="3">
@@ -2664,7 +2658,7 @@
         <v>1</v>
       </c>
       <c r="F57" s="3" t="b">
-        <f>ISNA(VLOOKUP(B57,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B57,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G57" s="3">
@@ -2694,7 +2688,7 @@
         <v>1</v>
       </c>
       <c r="F58" s="3" t="b">
-        <f>ISNA(VLOOKUP(B58,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B58,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G58" s="3">
@@ -2724,7 +2718,7 @@
         <v>1</v>
       </c>
       <c r="F59" s="3" t="b">
-        <f>ISNA(VLOOKUP(B59,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B59,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G59" s="3">
@@ -2754,7 +2748,7 @@
         <v>1</v>
       </c>
       <c r="F60" s="3" t="b">
-        <f>ISNA(VLOOKUP(B60,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B60,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G60" s="3">
@@ -2784,7 +2778,7 @@
         <v>1</v>
       </c>
       <c r="F61" s="3" t="b">
-        <f>ISNA(VLOOKUP(B61,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B61,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G61" s="3">
@@ -2814,7 +2808,7 @@
         <v>1</v>
       </c>
       <c r="F62" s="3" t="b">
-        <f>ISNA(VLOOKUP(B62,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B62,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G62" s="3">
@@ -2844,7 +2838,7 @@
         <v>1</v>
       </c>
       <c r="F63" s="3" t="b">
-        <f>ISNA(VLOOKUP(B63,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B63,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G63" s="3">
@@ -2874,7 +2868,7 @@
         <v>1</v>
       </c>
       <c r="F64" s="3" t="b">
-        <f>ISNA(VLOOKUP(B64,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B64,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G64" s="3">
@@ -2904,7 +2898,7 @@
         <v>1</v>
       </c>
       <c r="F65" s="3" t="b">
-        <f>ISNA(VLOOKUP(B65,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B65,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G65" s="3">
@@ -2934,7 +2928,7 @@
         <v>1</v>
       </c>
       <c r="F66" s="3" t="b">
-        <f>ISNA(VLOOKUP(B66,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B66,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G66" s="3">
@@ -2964,7 +2958,7 @@
         <v>1</v>
       </c>
       <c r="F67" s="3" t="b">
-        <f>ISNA(VLOOKUP(B67,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B67,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G67" s="3">
@@ -2994,7 +2988,7 @@
         <v>1</v>
       </c>
       <c r="F68" s="3" t="b">
-        <f>ISNA(VLOOKUP(B68,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B68,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G68" s="3">
@@ -3024,7 +3018,7 @@
         <v>1</v>
       </c>
       <c r="F69" s="3" t="b">
-        <f>ISNA(VLOOKUP(B69,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B69,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G69" s="3">
@@ -3054,7 +3048,7 @@
         <v>1</v>
       </c>
       <c r="F70" s="3" t="b">
-        <f>ISNA(VLOOKUP(B70,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B70,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G70" s="3">
@@ -3084,7 +3078,7 @@
         <v>1</v>
       </c>
       <c r="F71" s="3" t="b">
-        <f>ISNA(VLOOKUP(B71,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B71,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G71" s="3">
@@ -3114,7 +3108,7 @@
         <v>1</v>
       </c>
       <c r="F72" s="3" t="b">
-        <f>ISNA(VLOOKUP(B72,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B72,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G72" s="3">
@@ -3144,7 +3138,7 @@
         <v>1</v>
       </c>
       <c r="F73" s="3" t="b">
-        <f>ISNA(VLOOKUP(B73,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B73,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G73" s="3">
@@ -3174,7 +3168,7 @@
         <v>1</v>
       </c>
       <c r="F74" s="3" t="b">
-        <f>ISNA(VLOOKUP(B74,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B74,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G74" s="3">
@@ -3204,7 +3198,7 @@
         <v>1</v>
       </c>
       <c r="F75" s="3" t="b">
-        <f>ISNA(VLOOKUP(B75,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B75,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G75" s="3">
@@ -3234,7 +3228,7 @@
         <v>1</v>
       </c>
       <c r="F76" s="3" t="b">
-        <f>ISNA(VLOOKUP(B76,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B76,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G76" s="3">
@@ -3264,7 +3258,7 @@
         <v>1</v>
       </c>
       <c r="F77" s="3" t="b">
-        <f>ISNA(VLOOKUP(B77,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B77,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G77" s="3">
@@ -3294,7 +3288,7 @@
         <v>1</v>
       </c>
       <c r="F78" s="3" t="b">
-        <f>ISNA(VLOOKUP(B78,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B78,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G78" s="3">
@@ -3324,7 +3318,7 @@
         <v>1</v>
       </c>
       <c r="F79" s="3" t="b">
-        <f>ISNA(VLOOKUP(B79,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B79,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G79" s="3">
@@ -3354,7 +3348,7 @@
         <v>1</v>
       </c>
       <c r="F80" s="3" t="b">
-        <f>ISNA(VLOOKUP(B80,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B80,class2!$A$1:$B$86,2,FALSE))</f>
         <v>1</v>
       </c>
       <c r="G80" s="3">
@@ -3384,7 +3378,7 @@
         <v>1</v>
       </c>
       <c r="F81" s="3" t="b">
-        <f>ISNA(VLOOKUP(B81,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B81,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G81" s="3">
@@ -3414,7 +3408,7 @@
         <v>1</v>
       </c>
       <c r="F82" s="3" t="b">
-        <f>ISNA(VLOOKUP(B82,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B82,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G82" s="3">
@@ -3444,7 +3438,7 @@
         <v>1</v>
       </c>
       <c r="F83" s="3" t="b">
-        <f>ISNA(VLOOKUP(B83,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B83,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G83" s="3">
@@ -3474,7 +3468,7 @@
         <v>1</v>
       </c>
       <c r="F84" s="3" t="b">
-        <f>ISNA(VLOOKUP(B84,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B84,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G84" s="3">
@@ -3504,7 +3498,7 @@
         <v>1</v>
       </c>
       <c r="F85" s="3" t="b">
-        <f>ISNA(VLOOKUP(B85,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B85,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G85" s="3">
@@ -3534,7 +3528,7 @@
         <v>1</v>
       </c>
       <c r="F86" s="3" t="b">
-        <f>ISNA(VLOOKUP(B86,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B86,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G86" s="3">
@@ -3564,12 +3558,12 @@
         <v>1</v>
       </c>
       <c r="F87" s="3" t="b">
-        <f>ISNA(VLOOKUP(B87,class2!$A$1:$B$83,2,FALSE))</f>
-        <v>1</v>
+        <f>ISNA(VLOOKUP(B87,class2!$A$1:$B$86,2,FALSE))</f>
+        <v>0</v>
       </c>
       <c r="G87" s="3">
         <f t="shared" si="1"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="H87" s="3"/>
       <c r="I87" s="3"/>
@@ -3594,7 +3588,7 @@
         <v>1</v>
       </c>
       <c r="F88" s="3" t="b">
-        <f>ISNA(VLOOKUP(B88,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B88,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G88" s="3">
@@ -3624,7 +3618,7 @@
         <v>1</v>
       </c>
       <c r="F89" s="3" t="b">
-        <f>ISNA(VLOOKUP(B89,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B89,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G89" s="3">
@@ -3654,7 +3648,7 @@
         <v>1</v>
       </c>
       <c r="F90" s="3" t="b">
-        <f>ISNA(VLOOKUP(B90,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B90,class2!$A$1:$B$86,2,FALSE))</f>
         <v>1</v>
       </c>
       <c r="G90" s="3">
@@ -3684,7 +3678,7 @@
         <v>1</v>
       </c>
       <c r="F91" s="3" t="b">
-        <f>ISNA(VLOOKUP(B91,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B91,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G91" s="3">
@@ -3714,7 +3708,7 @@
         <v>1</v>
       </c>
       <c r="F92" s="3" t="b">
-        <f>ISNA(VLOOKUP(B92,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B92,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G92" s="3">
@@ -3744,7 +3738,7 @@
         <v>1</v>
       </c>
       <c r="F93" s="3" t="b">
-        <f>ISNA(VLOOKUP(B93,class2!$A$1:$B$83,2,FALSE))</f>
+        <f>ISNA(VLOOKUP(B93,class2!$A$1:$B$86,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="G93" s="3">
@@ -3794,10 +3788,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C83"/>
+  <dimension ref="A1:C85"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="F86" sqref="F86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4801,6 +4795,30 @@
         <v>市场营销15</v>
       </c>
     </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A84" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B84">
+        <v>1</v>
+      </c>
+      <c r="C84" t="str">
+        <f>VLOOKUP(A84,sum!$B$5:$C$93,2,FALSE)</f>
+        <v>大数据营销15</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A85" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B85">
+        <v>1</v>
+      </c>
+      <c r="C85" t="str">
+        <f>VLOOKUP(A85,sum!$B$5:$C$93,2,FALSE)</f>
+        <v>双培大数据营销15</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4809,463 +4827,14 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A89"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A89"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A32" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" s="3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" s="3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A38" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A41" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A42" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A43" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A44" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A45" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A46" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A47" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A48" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A49" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A50" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A51" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A52" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A53" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A54" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A55" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A56" s="3" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A57" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A58" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A59" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A60" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A61" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A62" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A63" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A64" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A65" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A66" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A67" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A68" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A69" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A70" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A71" s="17" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A72" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A73" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A74" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A75" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A76" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A77" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A78" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A79" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A80" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A81" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A82" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A83" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A84" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A85" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A86" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A87" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A88" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A89" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-  </sheetData>
-  <sortState ref="A1:A89">
-    <sortCondition ref="A1"/>
-  </sortState>
+  <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update the score file
</commit_message>
<xml_diff>
--- a/Materials/大数据菁英班成绩单（第一学期）.xlsx
+++ b/Materials/大数据菁英班成绩单（第一学期）.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28000" windowHeight="17540" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28000" windowHeight="17540"/>
   </bookViews>
   <sheets>
     <sheet name="sum" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="292">
   <si>
     <t>李婉荣</t>
   </si>
@@ -350,10 +350,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>备注</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>出勤情况</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -426,6 +422,516 @@
   </si>
   <si>
     <t>请假</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>2016/5/8 17:19:20</t>
+  </si>
+  <si>
+    <t>280秒</t>
+  </si>
+  <si>
+    <t>2016/5/8 17:19:28</t>
+  </si>
+  <si>
+    <t>282秒</t>
+  </si>
+  <si>
+    <t>2016/5/8 17:19:40</t>
+  </si>
+  <si>
+    <t>305秒</t>
+  </si>
+  <si>
+    <t>2016/5/8 17:19:48</t>
+  </si>
+  <si>
+    <t>312秒</t>
+  </si>
+  <si>
+    <t>2016/5/8 17:19:51</t>
+  </si>
+  <si>
+    <t>2016/5/8 17:20:01</t>
+  </si>
+  <si>
+    <t>324秒</t>
+  </si>
+  <si>
+    <t>2016/5/8 17:20:11</t>
+  </si>
+  <si>
+    <t>331秒</t>
+  </si>
+  <si>
+    <t>2016/5/8 17:20:26</t>
+  </si>
+  <si>
+    <t>351秒</t>
+  </si>
+  <si>
+    <t>2016/5/8 17:20:36</t>
+  </si>
+  <si>
+    <t>355秒</t>
+  </si>
+  <si>
+    <t>2016/5/8 17:20:39</t>
+  </si>
+  <si>
+    <t>353秒</t>
+  </si>
+  <si>
+    <t>2016/5/8 17:20:50</t>
+  </si>
+  <si>
+    <t>371秒</t>
+  </si>
+  <si>
+    <t>2016/5/8 17:20:51</t>
+  </si>
+  <si>
+    <t>2016/5/8 17:21:13</t>
+  </si>
+  <si>
+    <t>387秒</t>
+  </si>
+  <si>
+    <t>2016/5/8 17:21:21</t>
+  </si>
+  <si>
+    <t>400秒</t>
+  </si>
+  <si>
+    <t>2016/5/8 17:21:26</t>
+  </si>
+  <si>
+    <t>404秒</t>
+  </si>
+  <si>
+    <t>2016/5/8 17:21:28</t>
+  </si>
+  <si>
+    <t>406秒</t>
+  </si>
+  <si>
+    <t>2016/5/8 17:21:30</t>
+  </si>
+  <si>
+    <t>381秒</t>
+  </si>
+  <si>
+    <t>2016/5/8 17:21:37</t>
+  </si>
+  <si>
+    <t>420秒</t>
+  </si>
+  <si>
+    <t>2016/5/8 17:21:39</t>
+  </si>
+  <si>
+    <t>403秒</t>
+  </si>
+  <si>
+    <t>2016/5/8 17:21:40</t>
+  </si>
+  <si>
+    <t>424秒</t>
+  </si>
+  <si>
+    <t>421秒</t>
+  </si>
+  <si>
+    <t>2016/5/8 17:21:42</t>
+  </si>
+  <si>
+    <t>368秒</t>
+  </si>
+  <si>
+    <t>2016/5/8 17:21:43</t>
+  </si>
+  <si>
+    <t>426秒</t>
+  </si>
+  <si>
+    <t>419秒</t>
+  </si>
+  <si>
+    <t>2016/5/8 17:21:44</t>
+  </si>
+  <si>
+    <t>422秒</t>
+  </si>
+  <si>
+    <t>2016/5/8 17:21:46</t>
+  </si>
+  <si>
+    <t>427秒</t>
+  </si>
+  <si>
+    <t>2016/5/8 17:21:50</t>
+  </si>
+  <si>
+    <t>432秒</t>
+  </si>
+  <si>
+    <t>435秒</t>
+  </si>
+  <si>
+    <t>2016/5/8 17:21:56</t>
+  </si>
+  <si>
+    <t>430秒</t>
+  </si>
+  <si>
+    <t>2016/5/8 17:21:59</t>
+  </si>
+  <si>
+    <t>443秒</t>
+  </si>
+  <si>
+    <t>2016/5/8 17:22:04</t>
+  </si>
+  <si>
+    <t>442秒</t>
+  </si>
+  <si>
+    <t>2016/5/8 17:22:05</t>
+  </si>
+  <si>
+    <t>448秒</t>
+  </si>
+  <si>
+    <t>2016/5/8 17:22:07</t>
+  </si>
+  <si>
+    <t>307秒</t>
+  </si>
+  <si>
+    <t>2016/5/8 17:22:09</t>
+  </si>
+  <si>
+    <t>450秒</t>
+  </si>
+  <si>
+    <t>2016/5/8 17:22:21</t>
+  </si>
+  <si>
+    <t>461秒</t>
+  </si>
+  <si>
+    <t>2016/5/8 17:22:24</t>
+  </si>
+  <si>
+    <t>463秒</t>
+  </si>
+  <si>
+    <t>2016/5/8 17:22:26</t>
+  </si>
+  <si>
+    <t>468秒</t>
+  </si>
+  <si>
+    <t>2016/5/8 17:22:29</t>
+  </si>
+  <si>
+    <t>472秒</t>
+  </si>
+  <si>
+    <t>2016/5/8 17:22:31</t>
+  </si>
+  <si>
+    <t>474秒</t>
+  </si>
+  <si>
+    <t>2016/5/8 17:22:33</t>
+  </si>
+  <si>
+    <t>473秒</t>
+  </si>
+  <si>
+    <t>2016/5/8 17:22:34</t>
+  </si>
+  <si>
+    <t>471秒</t>
+  </si>
+  <si>
+    <t>2016/5/8 17:22:38</t>
+  </si>
+  <si>
+    <t>457秒</t>
+  </si>
+  <si>
+    <t>2016/5/8 17:22:40</t>
+  </si>
+  <si>
+    <t>483秒</t>
+  </si>
+  <si>
+    <t>2016/5/8 17:22:41</t>
+  </si>
+  <si>
+    <t>425秒</t>
+  </si>
+  <si>
+    <t>2016/5/8 17:22:42</t>
+  </si>
+  <si>
+    <t>481秒</t>
+  </si>
+  <si>
+    <t>2016/5/8 17:22:43</t>
+  </si>
+  <si>
+    <t>479秒</t>
+  </si>
+  <si>
+    <t>2016/5/8 17:22:45</t>
+  </si>
+  <si>
+    <t>418秒</t>
+  </si>
+  <si>
+    <t>2016/5/8 17:22:46</t>
+  </si>
+  <si>
+    <t>488秒</t>
+  </si>
+  <si>
+    <t>2016/5/8 17:22:48</t>
+  </si>
+  <si>
+    <t>491秒</t>
+  </si>
+  <si>
+    <t>490秒</t>
+  </si>
+  <si>
+    <t>2016/5/8 17:22:50</t>
+  </si>
+  <si>
+    <t>2016/5/8 17:22:51</t>
+  </si>
+  <si>
+    <t>494秒</t>
+  </si>
+  <si>
+    <t>2016/5/8 17:22:52</t>
+  </si>
+  <si>
+    <t>496秒</t>
+  </si>
+  <si>
+    <t>2016/5/8 17:22:57</t>
+  </si>
+  <si>
+    <t>500秒</t>
+  </si>
+  <si>
+    <t>2016/5/8 17:22:58</t>
+  </si>
+  <si>
+    <t>499秒</t>
+  </si>
+  <si>
+    <t>2016/5/8 17:22:59</t>
+  </si>
+  <si>
+    <t>501秒</t>
+  </si>
+  <si>
+    <t>2016/5/8 17:23:00</t>
+  </si>
+  <si>
+    <t>505秒</t>
+  </si>
+  <si>
+    <t>2016/5/8 17:23:03</t>
+  </si>
+  <si>
+    <t>2016/5/8 17:23:06</t>
+  </si>
+  <si>
+    <t>506秒</t>
+  </si>
+  <si>
+    <t>2016/5/8 17:23:08</t>
+  </si>
+  <si>
+    <t>508秒</t>
+  </si>
+  <si>
+    <t>2016/5/8 17:23:14</t>
+  </si>
+  <si>
+    <t>517秒</t>
+  </si>
+  <si>
+    <t>2016/5/8 17:23:20</t>
+  </si>
+  <si>
+    <t>52秒</t>
+  </si>
+  <si>
+    <t>2016/5/8 17:23:23</t>
+  </si>
+  <si>
+    <t>498秒</t>
+  </si>
+  <si>
+    <t>2016/5/8 17:23:27</t>
+  </si>
+  <si>
+    <t>504秒</t>
+  </si>
+  <si>
+    <t>2016/5/8 17:23:28</t>
+  </si>
+  <si>
+    <t>527秒</t>
+  </si>
+  <si>
+    <t>2016/5/8 17:23:38</t>
+  </si>
+  <si>
+    <t>541秒</t>
+  </si>
+  <si>
+    <t>2016/5/8 17:23:42</t>
+  </si>
+  <si>
+    <t>543秒</t>
+  </si>
+  <si>
+    <t>2016/5/8 17:23:47</t>
+  </si>
+  <si>
+    <t>2016/5/8 17:23:49</t>
+  </si>
+  <si>
+    <t>545秒</t>
+  </si>
+  <si>
+    <t>2016/5/8 17:23:53</t>
+  </si>
+  <si>
+    <t>549秒</t>
+  </si>
+  <si>
+    <t>2016/5/8 17:23:55</t>
+  </si>
+  <si>
+    <t>550秒</t>
+  </si>
+  <si>
+    <t>2016/5/8 17:24:01</t>
+  </si>
+  <si>
+    <t>2016/5/8 17:24:04</t>
+  </si>
+  <si>
+    <t>560秒</t>
+  </si>
+  <si>
+    <t>2016/5/8 17:24:10</t>
+  </si>
+  <si>
+    <t>551秒</t>
+  </si>
+  <si>
+    <t>2016/5/8 17:24:13</t>
+  </si>
+  <si>
+    <t>570秒</t>
+  </si>
+  <si>
+    <t>2016/5/8 17:24:14</t>
+  </si>
+  <si>
+    <t>574秒</t>
+  </si>
+  <si>
+    <t>2016/5/8 17:24:27</t>
+  </si>
+  <si>
+    <t>591秒</t>
+  </si>
+  <si>
+    <t>2016/5/8 17:24:56</t>
+  </si>
+  <si>
+    <t>97秒</t>
+  </si>
+  <si>
+    <t>2016/5/8 17:25:20</t>
+  </si>
+  <si>
+    <t>83秒</t>
+  </si>
+  <si>
+    <t>2016/5/8 17:25:47</t>
+  </si>
+  <si>
+    <t>669秒</t>
+  </si>
+  <si>
+    <t>2016/5/8 17:25:57</t>
+  </si>
+  <si>
+    <t>198秒</t>
+  </si>
+  <si>
+    <t>2016/5/8 17:26:27</t>
+  </si>
+  <si>
+    <t>124秒</t>
+  </si>
+  <si>
+    <t>2016/5/8 17:27:49</t>
+  </si>
+  <si>
+    <t>88秒</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>score</t>
+  </si>
+  <si>
+    <t>submittime</t>
+  </si>
+  <si>
+    <t>totaltime</t>
+  </si>
+  <si>
+    <t>bonus</t>
+  </si>
+  <si>
+    <t>final</t>
+  </si>
+  <si>
+    <t>总成绩</t>
   </si>
 </sst>
 </file>
@@ -639,7 +1145,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -690,6 +1196,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -994,8 +1503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L93"/>
   <sheetViews>
-    <sheetView topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="F57" sqref="F1:F1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1007,7 +1516,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B1" s="14"/>
       <c r="C1" s="14"/>
@@ -1023,7 +1532,7 @@
     </row>
     <row r="2" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -1039,7 +1548,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>87</v>
@@ -1048,7 +1557,7 @@
         <v>88</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E3" s="9"/>
       <c r="F3" s="9"/>
@@ -1070,17 +1579,19 @@
         <v>42469</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G4" s="7">
         <v>42483</v>
       </c>
-      <c r="H4" s="1"/>
+      <c r="H4" s="7">
+        <v>42498</v>
+      </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="2" t="s">
-        <v>98</v>
+        <v>291</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -1107,7 +1618,10 @@
         <f>IF(F5=FALSE,1,-1)</f>
         <v>1</v>
       </c>
-      <c r="H5" s="3"/>
+      <c r="H5" s="3">
+        <f>VLOOKUP(B5,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>60</v>
+      </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
@@ -1137,7 +1651,10 @@
         <f t="shared" ref="G6:G70" si="0">IF(F6=FALSE,1,-1)</f>
         <v>1</v>
       </c>
-      <c r="H6" s="3"/>
+      <c r="H6" s="3">
+        <f>VLOOKUP(B6,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>50</v>
+      </c>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
@@ -1167,7 +1684,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H7" s="3"/>
+      <c r="H7" s="3">
+        <f>VLOOKUP(B7,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>60</v>
+      </c>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
@@ -1197,7 +1717,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H8" s="3"/>
+      <c r="H8" s="3">
+        <f>VLOOKUP(B8,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>45</v>
+      </c>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
@@ -1227,7 +1750,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H9" s="3"/>
+      <c r="H9" s="3">
+        <f>VLOOKUP(B9,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>60</v>
+      </c>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
@@ -1257,7 +1783,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H10" s="3"/>
+      <c r="H10" s="3">
+        <f>VLOOKUP(B10,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>60</v>
+      </c>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
@@ -1287,7 +1816,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H11" s="3"/>
+      <c r="H11" s="3">
+        <f>VLOOKUP(B11,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>60</v>
+      </c>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
@@ -1317,7 +1849,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H12" s="3"/>
+      <c r="H12" s="3">
+        <f>VLOOKUP(B12,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>60</v>
+      </c>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
@@ -1347,7 +1882,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H13" s="3"/>
+      <c r="H13" s="3">
+        <f>VLOOKUP(B13,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>50</v>
+      </c>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
@@ -1377,7 +1915,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H14" s="3"/>
+      <c r="H14" s="3">
+        <f>VLOOKUP(B14,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>60</v>
+      </c>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
@@ -1400,12 +1941,15 @@
         <v>1</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G15" s="3">
         <v>0</v>
       </c>
-      <c r="H15" s="3"/>
+      <c r="H15" s="3">
+        <f>VLOOKUP(B15,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>60</v>
+      </c>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
@@ -1435,7 +1979,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H16" s="3"/>
+      <c r="H16" s="3">
+        <f>VLOOKUP(B16,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>35</v>
+      </c>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
@@ -1465,7 +2012,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H17" s="3"/>
+      <c r="H17" s="3">
+        <f>VLOOKUP(B17,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>50</v>
+      </c>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
@@ -1495,7 +2045,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H18" s="3"/>
+      <c r="H18" s="3">
+        <f>VLOOKUP(B18,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>60</v>
+      </c>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
@@ -1525,7 +2078,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H19" s="3"/>
+      <c r="H19" s="3">
+        <f>VLOOKUP(B19,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>40</v>
+      </c>
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
@@ -1555,7 +2111,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H20" s="3"/>
+      <c r="H20" s="3">
+        <f>VLOOKUP(B20,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>40</v>
+      </c>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
@@ -1585,7 +2144,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H21" s="3"/>
+      <c r="H21" s="3">
+        <f>VLOOKUP(B21,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>60</v>
+      </c>
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
@@ -1615,7 +2177,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H22" s="3"/>
+      <c r="H22" s="3">
+        <f>VLOOKUP(B22,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>55</v>
+      </c>
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
@@ -1645,7 +2210,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H23" s="3"/>
+      <c r="H23" s="3">
+        <f>VLOOKUP(B23,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>55</v>
+      </c>
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
@@ -1675,7 +2243,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H24" s="3"/>
+      <c r="H24" s="3">
+        <f>VLOOKUP(B24,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>55</v>
+      </c>
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
@@ -1705,7 +2276,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H25" s="3"/>
+      <c r="H25" s="3">
+        <f>VLOOKUP(B25,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>45</v>
+      </c>
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
@@ -1735,7 +2309,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H26" s="3"/>
+      <c r="H26" s="3">
+        <f>VLOOKUP(B26,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>55</v>
+      </c>
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
@@ -1765,7 +2342,10 @@
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="H27" s="3"/>
+      <c r="H27" s="3">
+        <f>VLOOKUP(B27,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>60</v>
+      </c>
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
@@ -1795,7 +2375,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H28" s="3"/>
+      <c r="H28" s="3">
+        <f>VLOOKUP(B28,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>55</v>
+      </c>
       <c r="I28" s="3"/>
       <c r="J28" s="3"/>
       <c r="K28" s="3"/>
@@ -1825,7 +2408,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H29" s="3"/>
+      <c r="H29" s="3">
+        <f>VLOOKUP(B29,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>45</v>
+      </c>
       <c r="I29" s="3"/>
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
@@ -1855,7 +2441,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H30" s="3"/>
+      <c r="H30" s="3">
+        <f>VLOOKUP(B30,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>55</v>
+      </c>
       <c r="I30" s="3"/>
       <c r="J30" s="3"/>
       <c r="K30" s="3"/>
@@ -1885,7 +2474,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H31" s="3"/>
+      <c r="H31" s="3">
+        <f>VLOOKUP(B31,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>45</v>
+      </c>
       <c r="I31" s="3"/>
       <c r="J31" s="3"/>
       <c r="K31" s="3"/>
@@ -1915,7 +2507,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H32" s="3"/>
+      <c r="H32" s="3" t="e">
+        <f>VLOOKUP(B32,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>#N/A</v>
+      </c>
       <c r="I32" s="3"/>
       <c r="J32" s="3"/>
       <c r="K32" s="3"/>
@@ -1945,7 +2540,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H33" s="3"/>
+      <c r="H33" s="3">
+        <f>VLOOKUP(B33,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>60</v>
+      </c>
       <c r="I33" s="3"/>
       <c r="J33" s="3"/>
       <c r="K33" s="3"/>
@@ -1975,7 +2573,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H34" s="3"/>
+      <c r="H34" s="3">
+        <f>VLOOKUP(B34,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>35</v>
+      </c>
       <c r="I34" s="3"/>
       <c r="J34" s="3"/>
       <c r="K34" s="3"/>
@@ -2005,7 +2606,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H35" s="3"/>
+      <c r="H35" s="3">
+        <f>VLOOKUP(B35,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>60</v>
+      </c>
       <c r="I35" s="3"/>
       <c r="J35" s="3"/>
       <c r="K35" s="3"/>
@@ -2035,7 +2639,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H36" s="3"/>
+      <c r="H36" s="3">
+        <f>VLOOKUP(B36,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>50</v>
+      </c>
       <c r="I36" s="3"/>
       <c r="J36" s="3"/>
       <c r="K36" s="3"/>
@@ -2065,7 +2672,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H37" s="3"/>
+      <c r="H37" s="3">
+        <f>VLOOKUP(B37,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>60</v>
+      </c>
       <c r="I37" s="3"/>
       <c r="J37" s="3"/>
       <c r="K37" s="3"/>
@@ -2095,7 +2705,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H38" s="3"/>
+      <c r="H38" s="3">
+        <f>VLOOKUP(B38,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>55</v>
+      </c>
       <c r="I38" s="3"/>
       <c r="J38" s="3"/>
       <c r="K38" s="3"/>
@@ -2125,7 +2738,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H39" s="3"/>
+      <c r="H39" s="3">
+        <f>VLOOKUP(B39,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>50</v>
+      </c>
       <c r="I39" s="3"/>
       <c r="J39" s="3"/>
       <c r="K39" s="3"/>
@@ -2155,7 +2771,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H40" s="3"/>
+      <c r="H40" s="3">
+        <f>VLOOKUP(B40,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>50</v>
+      </c>
       <c r="I40" s="3"/>
       <c r="J40" s="3"/>
       <c r="K40" s="3"/>
@@ -2185,7 +2804,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H41" s="3"/>
+      <c r="H41" s="3">
+        <f>VLOOKUP(B41,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>45</v>
+      </c>
       <c r="I41" s="3"/>
       <c r="J41" s="3"/>
       <c r="K41" s="3"/>
@@ -2215,7 +2837,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H42" s="3"/>
+      <c r="H42" s="3">
+        <f>VLOOKUP(B42,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>60</v>
+      </c>
       <c r="I42" s="3"/>
       <c r="J42" s="3"/>
       <c r="K42" s="3"/>
@@ -2226,7 +2851,7 @@
         <v>39</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>92</v>
@@ -2245,7 +2870,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H43" s="3"/>
+      <c r="H43" s="3">
+        <f>VLOOKUP(B43,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>50</v>
+      </c>
       <c r="I43" s="3"/>
       <c r="J43" s="3"/>
       <c r="K43" s="3"/>
@@ -2275,7 +2903,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H44" s="3"/>
+      <c r="H44" s="3">
+        <f>VLOOKUP(B44,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>55</v>
+      </c>
       <c r="I44" s="3"/>
       <c r="J44" s="3"/>
       <c r="K44" s="3"/>
@@ -2305,7 +2936,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H45" s="3"/>
+      <c r="H45" s="3">
+        <f>VLOOKUP(B45,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>55</v>
+      </c>
       <c r="I45" s="3"/>
       <c r="J45" s="3"/>
       <c r="K45" s="3"/>
@@ -2335,7 +2969,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H46" s="3"/>
+      <c r="H46" s="3">
+        <f>VLOOKUP(B46,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>55</v>
+      </c>
       <c r="I46" s="3"/>
       <c r="J46" s="3"/>
       <c r="K46" s="3"/>
@@ -2365,7 +3002,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H47" s="3"/>
+      <c r="H47" s="3">
+        <f>VLOOKUP(B47,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>60</v>
+      </c>
       <c r="I47" s="3"/>
       <c r="J47" s="3"/>
       <c r="K47" s="3"/>
@@ -2395,7 +3035,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H48" s="3"/>
+      <c r="H48" s="3">
+        <f>VLOOKUP(B48,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>55</v>
+      </c>
       <c r="I48" s="3"/>
       <c r="J48" s="3"/>
       <c r="K48" s="3"/>
@@ -2425,7 +3068,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H49" s="3"/>
+      <c r="H49" s="3">
+        <f>VLOOKUP(B49,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>65</v>
+      </c>
       <c r="I49" s="3"/>
       <c r="J49" s="3"/>
       <c r="K49" s="3"/>
@@ -2455,7 +3101,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H50" s="3"/>
+      <c r="H50" s="3">
+        <f>VLOOKUP(B50,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>60</v>
+      </c>
       <c r="I50" s="3"/>
       <c r="J50" s="3"/>
       <c r="K50" s="3"/>
@@ -2485,7 +3134,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H51" s="3"/>
+      <c r="H51" s="3">
+        <f>VLOOKUP(B51,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>55</v>
+      </c>
       <c r="I51" s="3"/>
       <c r="J51" s="3"/>
       <c r="K51" s="3"/>
@@ -2515,7 +3167,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H52" s="3"/>
+      <c r="H52" s="3">
+        <f>VLOOKUP(B52,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>65</v>
+      </c>
       <c r="I52" s="3"/>
       <c r="J52" s="3"/>
       <c r="K52" s="3"/>
@@ -2545,7 +3200,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H53" s="3"/>
+      <c r="H53" s="3">
+        <f>VLOOKUP(B53,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>60</v>
+      </c>
       <c r="I53" s="3"/>
       <c r="J53" s="3"/>
       <c r="K53" s="3"/>
@@ -2575,7 +3233,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H54" s="3"/>
+      <c r="H54" s="3">
+        <f>VLOOKUP(B54,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>60</v>
+      </c>
       <c r="I54" s="3"/>
       <c r="J54" s="3"/>
       <c r="K54" s="3"/>
@@ -2605,7 +3266,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H55" s="3"/>
+      <c r="H55" s="3">
+        <f>VLOOKUP(B55,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>60</v>
+      </c>
       <c r="I55" s="3"/>
       <c r="J55" s="3"/>
       <c r="K55" s="3"/>
@@ -2635,7 +3299,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H56" s="3"/>
+      <c r="H56" s="3">
+        <f>VLOOKUP(B56,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>60</v>
+      </c>
       <c r="I56" s="3"/>
       <c r="J56" s="3"/>
       <c r="K56" s="3"/>
@@ -2665,7 +3332,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H57" s="3"/>
+      <c r="H57" s="3">
+        <f>VLOOKUP(B57,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>65</v>
+      </c>
       <c r="I57" s="3"/>
       <c r="J57" s="3"/>
       <c r="K57" s="3"/>
@@ -2695,7 +3365,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H58" s="3"/>
+      <c r="H58" s="3">
+        <f>VLOOKUP(B58,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>55</v>
+      </c>
       <c r="I58" s="3"/>
       <c r="J58" s="3"/>
       <c r="K58" s="3"/>
@@ -2725,7 +3398,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H59" s="3"/>
+      <c r="H59" s="3">
+        <f>VLOOKUP(B59,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>60</v>
+      </c>
       <c r="I59" s="3"/>
       <c r="J59" s="3"/>
       <c r="K59" s="3"/>
@@ -2755,7 +3431,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H60" s="3"/>
+      <c r="H60" s="3">
+        <f>VLOOKUP(B60,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>65</v>
+      </c>
       <c r="I60" s="3"/>
       <c r="J60" s="3"/>
       <c r="K60" s="3"/>
@@ -2785,7 +3464,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H61" s="3"/>
+      <c r="H61" s="3">
+        <f>VLOOKUP(B61,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>65</v>
+      </c>
       <c r="I61" s="3"/>
       <c r="J61" s="3"/>
       <c r="K61" s="3"/>
@@ -2815,7 +3497,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H62" s="3"/>
+      <c r="H62" s="3">
+        <f>VLOOKUP(B62,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>50</v>
+      </c>
       <c r="I62" s="3"/>
       <c r="J62" s="3"/>
       <c r="K62" s="3"/>
@@ -2826,7 +3511,7 @@
         <v>59</v>
       </c>
       <c r="B63" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C63" s="3" t="s">
         <v>93</v>
@@ -2845,7 +3530,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H63" s="3"/>
+      <c r="H63" s="3">
+        <f>VLOOKUP(B63,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>60</v>
+      </c>
       <c r="I63" s="3"/>
       <c r="J63" s="3"/>
       <c r="K63" s="3"/>
@@ -2875,7 +3563,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H64" s="3"/>
+      <c r="H64" s="3">
+        <f>VLOOKUP(B64,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>55</v>
+      </c>
       <c r="I64" s="3"/>
       <c r="J64" s="3"/>
       <c r="K64" s="3"/>
@@ -2905,7 +3596,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H65" s="3"/>
+      <c r="H65" s="3">
+        <f>VLOOKUP(B65,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>50</v>
+      </c>
       <c r="I65" s="3"/>
       <c r="J65" s="3"/>
       <c r="K65" s="3"/>
@@ -2935,7 +3629,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H66" s="3"/>
+      <c r="H66" s="3">
+        <f>VLOOKUP(B66,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>55</v>
+      </c>
       <c r="I66" s="3"/>
       <c r="J66" s="3"/>
       <c r="K66" s="3"/>
@@ -2965,7 +3662,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H67" s="3"/>
+      <c r="H67" s="3">
+        <f>VLOOKUP(B67,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>50</v>
+      </c>
       <c r="I67" s="3"/>
       <c r="J67" s="3"/>
       <c r="K67" s="3"/>
@@ -2995,7 +3695,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H68" s="3"/>
+      <c r="H68" s="3">
+        <f>VLOOKUP(B68,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>55</v>
+      </c>
       <c r="I68" s="3"/>
       <c r="J68" s="3"/>
       <c r="K68" s="3"/>
@@ -3025,7 +3728,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H69" s="3"/>
+      <c r="H69" s="3">
+        <f>VLOOKUP(B69,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>40</v>
+      </c>
       <c r="I69" s="3"/>
       <c r="J69" s="3"/>
       <c r="K69" s="3"/>
@@ -3055,7 +3761,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H70" s="3"/>
+      <c r="H70" s="3">
+        <f>VLOOKUP(B70,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>45</v>
+      </c>
       <c r="I70" s="3"/>
       <c r="J70" s="3"/>
       <c r="K70" s="3"/>
@@ -3085,7 +3794,10 @@
         <f t="shared" ref="G71:G93" si="1">IF(F71=FALSE,1,-1)</f>
         <v>1</v>
       </c>
-      <c r="H71" s="3"/>
+      <c r="H71" s="3">
+        <f>VLOOKUP(B71,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>55</v>
+      </c>
       <c r="I71" s="3"/>
       <c r="J71" s="3"/>
       <c r="K71" s="3"/>
@@ -3115,7 +3827,10 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="H72" s="3"/>
+      <c r="H72" s="3">
+        <f>VLOOKUP(B72,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>50</v>
+      </c>
       <c r="I72" s="3"/>
       <c r="J72" s="3"/>
       <c r="K72" s="3"/>
@@ -3145,7 +3860,10 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="H73" s="3"/>
+      <c r="H73" s="3">
+        <f>VLOOKUP(B73,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>45</v>
+      </c>
       <c r="I73" s="3"/>
       <c r="J73" s="3"/>
       <c r="K73" s="3"/>
@@ -3175,7 +3893,10 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="H74" s="3"/>
+      <c r="H74" s="3">
+        <f>VLOOKUP(B74,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>55</v>
+      </c>
       <c r="I74" s="3"/>
       <c r="J74" s="3"/>
       <c r="K74" s="3"/>
@@ -3205,7 +3926,10 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="H75" s="3"/>
+      <c r="H75" s="3">
+        <f>VLOOKUP(B75,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>55</v>
+      </c>
       <c r="I75" s="3"/>
       <c r="J75" s="3"/>
       <c r="K75" s="3"/>
@@ -3235,7 +3959,10 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="H76" s="3"/>
+      <c r="H76" s="3">
+        <f>VLOOKUP(B76,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>45</v>
+      </c>
       <c r="I76" s="3"/>
       <c r="J76" s="3"/>
       <c r="K76" s="3"/>
@@ -3265,7 +3992,10 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="H77" s="3"/>
+      <c r="H77" s="3">
+        <f>VLOOKUP(B77,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>60</v>
+      </c>
       <c r="I77" s="3"/>
       <c r="J77" s="3"/>
       <c r="K77" s="3"/>
@@ -3295,7 +4025,10 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="H78" s="3"/>
+      <c r="H78" s="3">
+        <f>VLOOKUP(B78,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>55</v>
+      </c>
       <c r="I78" s="3"/>
       <c r="J78" s="3"/>
       <c r="K78" s="3"/>
@@ -3325,7 +4058,10 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="H79" s="3"/>
+      <c r="H79" s="3">
+        <f>VLOOKUP(B79,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>45</v>
+      </c>
       <c r="I79" s="3"/>
       <c r="J79" s="3"/>
       <c r="K79" s="3"/>
@@ -3355,7 +4091,10 @@
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="H80" s="3"/>
+      <c r="H80" s="3" t="e">
+        <f>VLOOKUP(B80,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>#N/A</v>
+      </c>
       <c r="I80" s="3"/>
       <c r="J80" s="3"/>
       <c r="K80" s="3"/>
@@ -3385,7 +4124,10 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="H81" s="3"/>
+      <c r="H81" s="3">
+        <f>VLOOKUP(B81,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>30</v>
+      </c>
       <c r="I81" s="3"/>
       <c r="J81" s="3"/>
       <c r="K81" s="3"/>
@@ -3415,7 +4157,10 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="H82" s="3"/>
+      <c r="H82" s="3">
+        <f>VLOOKUP(B82,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>45</v>
+      </c>
       <c r="I82" s="3"/>
       <c r="J82" s="3"/>
       <c r="K82" s="3"/>
@@ -3445,7 +4190,10 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="H83" s="3"/>
+      <c r="H83" s="3">
+        <f>VLOOKUP(B83,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>50</v>
+      </c>
       <c r="I83" s="3"/>
       <c r="J83" s="3"/>
       <c r="K83" s="3"/>
@@ -3475,7 +4223,10 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="H84" s="3"/>
+      <c r="H84" s="3">
+        <f>VLOOKUP(B84,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>55</v>
+      </c>
       <c r="I84" s="3"/>
       <c r="J84" s="3"/>
       <c r="K84" s="3"/>
@@ -3505,7 +4256,10 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="H85" s="3"/>
+      <c r="H85" s="3">
+        <f>VLOOKUP(B85,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>55</v>
+      </c>
       <c r="I85" s="3"/>
       <c r="J85" s="3"/>
       <c r="K85" s="3"/>
@@ -3535,7 +4289,10 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="H86" s="3"/>
+      <c r="H86" s="3">
+        <f>VLOOKUP(B86,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>50</v>
+      </c>
       <c r="I86" s="3"/>
       <c r="J86" s="3"/>
       <c r="K86" s="3"/>
@@ -3565,7 +4322,10 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="H87" s="3"/>
+      <c r="H87" s="3">
+        <f>VLOOKUP(B87,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>50</v>
+      </c>
       <c r="I87" s="3"/>
       <c r="J87" s="3"/>
       <c r="K87" s="3"/>
@@ -3595,7 +4355,10 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="H88" s="3"/>
+      <c r="H88" s="3">
+        <f>VLOOKUP(B88,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>45</v>
+      </c>
       <c r="I88" s="3"/>
       <c r="J88" s="3"/>
       <c r="K88" s="3"/>
@@ -3625,7 +4388,10 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="H89" s="3"/>
+      <c r="H89" s="3">
+        <f>VLOOKUP(B89,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>50</v>
+      </c>
       <c r="I89" s="3"/>
       <c r="J89" s="3"/>
       <c r="K89" s="3"/>
@@ -3655,7 +4421,10 @@
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="H90" s="3"/>
+      <c r="H90" s="3" t="e">
+        <f>VLOOKUP(B90,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>#N/A</v>
+      </c>
       <c r="I90" s="3"/>
       <c r="J90" s="3"/>
       <c r="K90" s="3"/>
@@ -3685,7 +4454,10 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="H91" s="3"/>
+      <c r="H91" s="3">
+        <f>VLOOKUP(B91,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>60</v>
+      </c>
       <c r="I91" s="3"/>
       <c r="J91" s="3"/>
       <c r="K91" s="3"/>
@@ -3715,7 +4487,10 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="H92" s="3"/>
+      <c r="H92" s="3">
+        <f>VLOOKUP(B92,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>60</v>
+      </c>
       <c r="I92" s="3"/>
       <c r="J92" s="3"/>
       <c r="K92" s="3"/>
@@ -3745,7 +4520,10 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="H93" s="5"/>
+      <c r="H93" s="3">
+        <f>VLOOKUP(B93,class3!$A$1:$F$90,6,FALSE)</f>
+        <v>55</v>
+      </c>
       <c r="I93" s="5"/>
       <c r="J93" s="5"/>
       <c r="K93" s="5"/>
@@ -3762,6 +4540,16 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="D3:G1048576">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="num" val="-1"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FF92D050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C97">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="num" val="-1"/>
@@ -3771,13 +4559,23 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C97">
-    <cfRule type="colorScale" priority="1">
+  <conditionalFormatting sqref="H4">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="num" val="-1"/>
         <cfvo type="num" val="1"/>
         <color rgb="FFFF7128"/>
         <color rgb="FF92D050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H5:H93">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FF00B050"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
@@ -3897,7 +4695,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -3981,7 +4779,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -4005,7 +4803,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -4053,7 +4851,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -4173,7 +4971,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -4293,7 +5091,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B42">
         <v>1</v>
@@ -4305,7 +5103,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B43">
         <v>1</v>
@@ -4329,7 +5127,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B45">
         <v>1</v>
@@ -4389,7 +5187,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B50">
         <v>1</v>
@@ -4401,7 +5199,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B51">
         <v>1</v>
@@ -4485,7 +5283,7 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B58">
         <v>1</v>
@@ -4509,7 +5307,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B60">
         <v>1</v>
@@ -4677,7 +5475,7 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B74">
         <v>1</v>
@@ -4725,7 +5523,7 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B78">
         <v>1</v>
@@ -4737,7 +5535,7 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B79">
         <v>1</v>
@@ -4749,7 +5547,7 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B80">
         <v>1</v>
@@ -4761,7 +5559,7 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B81">
         <v>1</v>
@@ -4785,7 +5583,7 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B83">
         <v>1</v>
@@ -4827,14 +5625,1619 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F87"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+    <sheetView topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="H81" sqref="H81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="12.6640625" customWidth="1"/>
+    <col min="2" max="2" width="4.1640625" customWidth="1"/>
+    <col min="3" max="3" width="16.1640625" customWidth="1"/>
+    <col min="4" max="4" width="7" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>285</v>
+      </c>
+      <c r="B1" t="s">
+        <v>286</v>
+      </c>
+      <c r="C1" t="s">
+        <v>287</v>
+      </c>
+      <c r="D1" t="s">
+        <v>288</v>
+      </c>
+      <c r="E1" t="s">
+        <v>289</v>
+      </c>
+      <c r="F1" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
+      <c r="F2">
+        <f>B2+E2</f>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C3" t="s">
+        <v>131</v>
+      </c>
+      <c r="D3" t="s">
+        <v>132</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F66" si="0">B3+E3</f>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C4" t="s">
+        <v>133</v>
+      </c>
+      <c r="D4" t="s">
+        <v>134</v>
+      </c>
+      <c r="E4">
+        <v>5</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" t="s">
+        <v>123</v>
+      </c>
+      <c r="C5" t="s">
+        <v>135</v>
+      </c>
+      <c r="D5" t="s">
+        <v>136</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>124</v>
+      </c>
+      <c r="C6" t="s">
+        <v>137</v>
+      </c>
+      <c r="D6" t="s">
+        <v>136</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" t="s">
+        <v>122</v>
+      </c>
+      <c r="C7" t="s">
+        <v>138</v>
+      </c>
+      <c r="D7" t="s">
+        <v>139</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>124</v>
+      </c>
+      <c r="C8" t="s">
+        <v>140</v>
+      </c>
+      <c r="D8" t="s">
+        <v>141</v>
+      </c>
+      <c r="E8">
+        <v>5</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" t="s">
+        <v>122</v>
+      </c>
+      <c r="C9" t="s">
+        <v>142</v>
+      </c>
+      <c r="D9" t="s">
+        <v>143</v>
+      </c>
+      <c r="E9">
+        <v>5</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>107</v>
+      </c>
+      <c r="B10" t="s">
+        <v>123</v>
+      </c>
+      <c r="C10" t="s">
+        <v>144</v>
+      </c>
+      <c r="D10" t="s">
+        <v>145</v>
+      </c>
+      <c r="E10">
+        <v>5</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C11" t="s">
+        <v>146</v>
+      </c>
+      <c r="D11" t="s">
+        <v>147</v>
+      </c>
+      <c r="E11">
+        <v>5</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" t="s">
+        <v>122</v>
+      </c>
+      <c r="C12" t="s">
+        <v>148</v>
+      </c>
+      <c r="D12" t="s">
+        <v>149</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>115</v>
+      </c>
+      <c r="B13" t="s">
+        <v>122</v>
+      </c>
+      <c r="C13" t="s">
+        <v>150</v>
+      </c>
+      <c r="D13" t="s">
+        <v>149</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>108</v>
+      </c>
+      <c r="B14" t="s">
+        <v>123</v>
+      </c>
+      <c r="C14" t="s">
+        <v>151</v>
+      </c>
+      <c r="D14" t="s">
+        <v>152</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" t="s">
+        <v>123</v>
+      </c>
+      <c r="C15" t="s">
+        <v>153</v>
+      </c>
+      <c r="D15" t="s">
+        <v>154</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" t="s">
+        <v>122</v>
+      </c>
+      <c r="C16" t="s">
+        <v>155</v>
+      </c>
+      <c r="D16" t="s">
+        <v>156</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>81</v>
+      </c>
+      <c r="B17" t="s">
+        <v>123</v>
+      </c>
+      <c r="C17" t="s">
+        <v>157</v>
+      </c>
+      <c r="D17" t="s">
+        <v>158</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>69</v>
+      </c>
+      <c r="B18" t="s">
+        <v>124</v>
+      </c>
+      <c r="C18" t="s">
+        <v>159</v>
+      </c>
+      <c r="D18" t="s">
+        <v>160</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" t="s">
+        <v>124</v>
+      </c>
+      <c r="C19" t="s">
+        <v>161</v>
+      </c>
+      <c r="D19" t="s">
+        <v>162</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" t="s">
+        <v>123</v>
+      </c>
+      <c r="C20" t="s">
+        <v>163</v>
+      </c>
+      <c r="D20" t="s">
+        <v>164</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" t="s">
+        <v>125</v>
+      </c>
+      <c r="C21" t="s">
+        <v>165</v>
+      </c>
+      <c r="D21" t="s">
+        <v>162</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>104</v>
+      </c>
+      <c r="B22" t="s">
+        <v>122</v>
+      </c>
+      <c r="C22" t="s">
+        <v>165</v>
+      </c>
+      <c r="D22" t="s">
+        <v>166</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" t="s">
+        <v>126</v>
+      </c>
+      <c r="C23" t="s">
+        <v>165</v>
+      </c>
+      <c r="D23" t="s">
+        <v>167</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>76</v>
+      </c>
+      <c r="B24" t="s">
+        <v>124</v>
+      </c>
+      <c r="C24" t="s">
+        <v>168</v>
+      </c>
+      <c r="D24" t="s">
+        <v>169</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>62</v>
+      </c>
+      <c r="B25" t="s">
+        <v>124</v>
+      </c>
+      <c r="C25" t="s">
+        <v>168</v>
+      </c>
+      <c r="D25" t="s">
+        <v>167</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>3</v>
+      </c>
+      <c r="B26" t="s">
+        <v>122</v>
+      </c>
+      <c r="C26" t="s">
+        <v>170</v>
+      </c>
+      <c r="D26" t="s">
+        <v>171</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>102</v>
+      </c>
+      <c r="B27" t="s">
+        <v>124</v>
+      </c>
+      <c r="C27" t="s">
+        <v>170</v>
+      </c>
+      <c r="D27" t="s">
+        <v>172</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" t="s">
+        <v>122</v>
+      </c>
+      <c r="C28" t="s">
+        <v>173</v>
+      </c>
+      <c r="D28" t="s">
+        <v>174</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>111</v>
+      </c>
+      <c r="B29" t="s">
+        <v>122</v>
+      </c>
+      <c r="C29" t="s">
+        <v>175</v>
+      </c>
+      <c r="D29" t="s">
+        <v>176</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>40</v>
+      </c>
+      <c r="B30" t="s">
+        <v>122</v>
+      </c>
+      <c r="C30" t="s">
+        <v>177</v>
+      </c>
+      <c r="D30" t="s">
+        <v>178</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>105</v>
+      </c>
+      <c r="B31" t="s">
+        <v>124</v>
+      </c>
+      <c r="C31" t="s">
+        <v>177</v>
+      </c>
+      <c r="D31" t="s">
+        <v>179</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>100</v>
+      </c>
+      <c r="B32" t="s">
+        <v>123</v>
+      </c>
+      <c r="C32" t="s">
+        <v>180</v>
+      </c>
+      <c r="D32" t="s">
+        <v>181</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>45</v>
+      </c>
+      <c r="B33" t="s">
+        <v>122</v>
+      </c>
+      <c r="C33" t="s">
+        <v>182</v>
+      </c>
+      <c r="D33" t="s">
+        <v>183</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>116</v>
+      </c>
+      <c r="B34" t="s">
+        <v>125</v>
+      </c>
+      <c r="C34" t="s">
+        <v>184</v>
+      </c>
+      <c r="D34" t="s">
+        <v>185</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>29</v>
+      </c>
+      <c r="B35" t="s">
+        <v>122</v>
+      </c>
+      <c r="C35" t="s">
+        <v>186</v>
+      </c>
+      <c r="D35" t="s">
+        <v>187</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>106</v>
+      </c>
+      <c r="B36" t="s">
+        <v>122</v>
+      </c>
+      <c r="C36" t="s">
+        <v>188</v>
+      </c>
+      <c r="D36" t="s">
+        <v>189</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>13</v>
+      </c>
+      <c r="B37" t="s">
+        <v>127</v>
+      </c>
+      <c r="C37" t="s">
+        <v>190</v>
+      </c>
+      <c r="D37" t="s">
+        <v>191</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>61</v>
+      </c>
+      <c r="B38" t="s">
+        <v>125</v>
+      </c>
+      <c r="C38" t="s">
+        <v>192</v>
+      </c>
+      <c r="D38" t="s">
+        <v>193</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>7</v>
+      </c>
+      <c r="B39" t="s">
+        <v>123</v>
+      </c>
+      <c r="C39" t="s">
+        <v>194</v>
+      </c>
+      <c r="D39" t="s">
+        <v>195</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>31</v>
+      </c>
+      <c r="B40" t="s">
+        <v>124</v>
+      </c>
+      <c r="C40" t="s">
+        <v>196</v>
+      </c>
+      <c r="D40" t="s">
+        <v>197</v>
+      </c>
+      <c r="F40">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>101</v>
+      </c>
+      <c r="B41" t="s">
+        <v>124</v>
+      </c>
+      <c r="C41" t="s">
+        <v>198</v>
+      </c>
+      <c r="D41" t="s">
+        <v>199</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>109</v>
+      </c>
+      <c r="B42" t="s">
+        <v>124</v>
+      </c>
+      <c r="C42" t="s">
+        <v>200</v>
+      </c>
+      <c r="D42" t="s">
+        <v>201</v>
+      </c>
+      <c r="F42">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>15</v>
+      </c>
+      <c r="B43" t="s">
+        <v>122</v>
+      </c>
+      <c r="C43" t="s">
+        <v>202</v>
+      </c>
+      <c r="D43" t="s">
+        <v>203</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>56</v>
+      </c>
+      <c r="B44" t="s">
+        <v>123</v>
+      </c>
+      <c r="C44" t="s">
+        <v>204</v>
+      </c>
+      <c r="D44" t="s">
+        <v>205</v>
+      </c>
+      <c r="F44">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>65</v>
+      </c>
+      <c r="B45" t="s">
+        <v>125</v>
+      </c>
+      <c r="C45" t="s">
+        <v>206</v>
+      </c>
+      <c r="D45" t="s">
+        <v>207</v>
+      </c>
+      <c r="F45">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>72</v>
+      </c>
+      <c r="B46" t="s">
+        <v>128</v>
+      </c>
+      <c r="C46" t="s">
+        <v>208</v>
+      </c>
+      <c r="D46" t="s">
+        <v>201</v>
+      </c>
+      <c r="F46">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>36</v>
+      </c>
+      <c r="B47" t="s">
+        <v>122</v>
+      </c>
+      <c r="C47" t="s">
+        <v>208</v>
+      </c>
+      <c r="D47" t="s">
+        <v>209</v>
+      </c>
+      <c r="F47">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>6</v>
+      </c>
+      <c r="B48" t="s">
+        <v>122</v>
+      </c>
+      <c r="C48" t="s">
+        <v>210</v>
+      </c>
+      <c r="D48" t="s">
+        <v>211</v>
+      </c>
+      <c r="F48">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>63</v>
+      </c>
+      <c r="B49" t="s">
+        <v>123</v>
+      </c>
+      <c r="C49" t="s">
+        <v>212</v>
+      </c>
+      <c r="D49" t="s">
+        <v>213</v>
+      </c>
+      <c r="F49">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>117</v>
+      </c>
+      <c r="B50" t="s">
+        <v>122</v>
+      </c>
+      <c r="C50" t="s">
+        <v>214</v>
+      </c>
+      <c r="D50" t="s">
+        <v>215</v>
+      </c>
+      <c r="F50">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>11</v>
+      </c>
+      <c r="B51" t="s">
+        <v>123</v>
+      </c>
+      <c r="C51" t="s">
+        <v>216</v>
+      </c>
+      <c r="D51" t="s">
+        <v>217</v>
+      </c>
+      <c r="F51">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>18</v>
+      </c>
+      <c r="B52" t="s">
+        <v>124</v>
+      </c>
+      <c r="C52" t="s">
+        <v>218</v>
+      </c>
+      <c r="D52" t="s">
+        <v>219</v>
+      </c>
+      <c r="F52">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>25</v>
+      </c>
+      <c r="B53" t="s">
+        <v>125</v>
+      </c>
+      <c r="C53" t="s">
+        <v>220</v>
+      </c>
+      <c r="D53" t="s">
+        <v>221</v>
+      </c>
+      <c r="F53">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>30</v>
+      </c>
+      <c r="B54" t="s">
+        <v>122</v>
+      </c>
+      <c r="C54" t="s">
+        <v>220</v>
+      </c>
+      <c r="D54" t="s">
+        <v>222</v>
+      </c>
+      <c r="F54">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>84</v>
+      </c>
+      <c r="B55" t="s">
+        <v>122</v>
+      </c>
+      <c r="C55" t="s">
+        <v>223</v>
+      </c>
+      <c r="D55" t="s">
+        <v>209</v>
+      </c>
+      <c r="F55">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>51</v>
+      </c>
+      <c r="B56" t="s">
+        <v>122</v>
+      </c>
+      <c r="C56" t="s">
+        <v>224</v>
+      </c>
+      <c r="D56" t="s">
+        <v>225</v>
+      </c>
+      <c r="F56">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>58</v>
+      </c>
+      <c r="B57" t="s">
+        <v>123</v>
+      </c>
+      <c r="C57" t="s">
+        <v>226</v>
+      </c>
+      <c r="D57" t="s">
+        <v>227</v>
+      </c>
+      <c r="F57">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>44</v>
+      </c>
+      <c r="B58" t="s">
+        <v>124</v>
+      </c>
+      <c r="C58" t="s">
+        <v>228</v>
+      </c>
+      <c r="D58" t="s">
+        <v>229</v>
+      </c>
+      <c r="F58">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>37</v>
+      </c>
+      <c r="B59" t="s">
+        <v>124</v>
+      </c>
+      <c r="C59" t="s">
+        <v>230</v>
+      </c>
+      <c r="D59" t="s">
+        <v>231</v>
+      </c>
+      <c r="F59">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>48</v>
+      </c>
+      <c r="B60" t="s">
+        <v>122</v>
+      </c>
+      <c r="C60" t="s">
+        <v>232</v>
+      </c>
+      <c r="D60" t="s">
+        <v>233</v>
+      </c>
+      <c r="F60">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>46</v>
+      </c>
+      <c r="B61" t="s">
+        <v>122</v>
+      </c>
+      <c r="C61" t="s">
+        <v>234</v>
+      </c>
+      <c r="D61" t="s">
+        <v>235</v>
+      </c>
+      <c r="F61">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>47</v>
+      </c>
+      <c r="B62" t="s">
+        <v>122</v>
+      </c>
+      <c r="C62" t="s">
+        <v>236</v>
+      </c>
+      <c r="D62" t="s">
+        <v>235</v>
+      </c>
+      <c r="F62">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>110</v>
+      </c>
+      <c r="B63" t="s">
+        <v>125</v>
+      </c>
+      <c r="C63" t="s">
+        <v>237</v>
+      </c>
+      <c r="D63" t="s">
+        <v>238</v>
+      </c>
+      <c r="F63">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>67</v>
+      </c>
+      <c r="B64" t="s">
+        <v>124</v>
+      </c>
+      <c r="C64" t="s">
+        <v>239</v>
+      </c>
+      <c r="D64" t="s">
+        <v>240</v>
+      </c>
+      <c r="F64">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>10</v>
+      </c>
+      <c r="B65" t="s">
+        <v>126</v>
+      </c>
+      <c r="C65" t="s">
+        <v>241</v>
+      </c>
+      <c r="D65" t="s">
+        <v>242</v>
+      </c>
+      <c r="F65">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A66" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="B66" t="s">
+        <v>123</v>
+      </c>
+      <c r="C66" t="s">
+        <v>243</v>
+      </c>
+      <c r="D66" t="s">
+        <v>244</v>
+      </c>
+      <c r="F66">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>38</v>
+      </c>
+      <c r="B67" t="s">
+        <v>124</v>
+      </c>
+      <c r="C67" t="s">
+        <v>245</v>
+      </c>
+      <c r="D67" t="s">
+        <v>246</v>
+      </c>
+      <c r="F67">
+        <f t="shared" ref="F67:F87" si="1">B67+E67</f>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>75</v>
+      </c>
+      <c r="B68" t="s">
+        <v>123</v>
+      </c>
+      <c r="C68" t="s">
+        <v>247</v>
+      </c>
+      <c r="D68" t="s">
+        <v>248</v>
+      </c>
+      <c r="F68">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>2</v>
+      </c>
+      <c r="B69" t="s">
+        <v>125</v>
+      </c>
+      <c r="C69" t="s">
+        <v>249</v>
+      </c>
+      <c r="D69" t="s">
+        <v>250</v>
+      </c>
+      <c r="F69">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>19</v>
+      </c>
+      <c r="B70" t="s">
+        <v>125</v>
+      </c>
+      <c r="C70" t="s">
+        <v>251</v>
+      </c>
+      <c r="D70" t="s">
+        <v>252</v>
+      </c>
+      <c r="F70">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>22</v>
+      </c>
+      <c r="B71" t="s">
+        <v>124</v>
+      </c>
+      <c r="C71" t="s">
+        <v>253</v>
+      </c>
+      <c r="D71" t="s">
+        <v>254</v>
+      </c>
+      <c r="F71">
+        <f t="shared" si="1"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>60</v>
+      </c>
+      <c r="B72" t="s">
+        <v>124</v>
+      </c>
+      <c r="C72" t="s">
+        <v>255</v>
+      </c>
+      <c r="D72" t="s">
+        <v>254</v>
+      </c>
+      <c r="F72">
+        <f t="shared" si="1"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>57</v>
+      </c>
+      <c r="B73" t="s">
+        <v>124</v>
+      </c>
+      <c r="C73" t="s">
+        <v>256</v>
+      </c>
+      <c r="D73" t="s">
+        <v>257</v>
+      </c>
+      <c r="F73">
+        <f t="shared" si="1"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>113</v>
+      </c>
+      <c r="B74" t="s">
+        <v>124</v>
+      </c>
+      <c r="C74" t="s">
+        <v>258</v>
+      </c>
+      <c r="D74" t="s">
+        <v>259</v>
+      </c>
+      <c r="F74">
+        <f t="shared" si="1"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>70</v>
+      </c>
+      <c r="B75" t="s">
+        <v>125</v>
+      </c>
+      <c r="C75" t="s">
+        <v>260</v>
+      </c>
+      <c r="D75" t="s">
+        <v>261</v>
+      </c>
+      <c r="F75">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>20</v>
+      </c>
+      <c r="B76" t="s">
+        <v>124</v>
+      </c>
+      <c r="C76" t="s">
+        <v>262</v>
+      </c>
+      <c r="D76" t="s">
+        <v>231</v>
+      </c>
+      <c r="F76">
+        <f t="shared" si="1"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>80</v>
+      </c>
+      <c r="B77" t="s">
+        <v>125</v>
+      </c>
+      <c r="C77" t="s">
+        <v>263</v>
+      </c>
+      <c r="D77" t="s">
+        <v>264</v>
+      </c>
+      <c r="F77">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>112</v>
+      </c>
+      <c r="B78" t="s">
+        <v>127</v>
+      </c>
+      <c r="C78" t="s">
+        <v>265</v>
+      </c>
+      <c r="D78" t="s">
+        <v>266</v>
+      </c>
+      <c r="F78">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>17</v>
+      </c>
+      <c r="B79" t="s">
+        <v>124</v>
+      </c>
+      <c r="C79" t="s">
+        <v>267</v>
+      </c>
+      <c r="D79" t="s">
+        <v>268</v>
+      </c>
+      <c r="F79">
+        <f t="shared" si="1"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>79</v>
+      </c>
+      <c r="B80" t="s">
+        <v>123</v>
+      </c>
+      <c r="C80" t="s">
+        <v>269</v>
+      </c>
+      <c r="D80" t="s">
+        <v>270</v>
+      </c>
+      <c r="F80">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>74</v>
+      </c>
+      <c r="B81" t="s">
+        <v>125</v>
+      </c>
+      <c r="C81" t="s">
+        <v>271</v>
+      </c>
+      <c r="D81" t="s">
+        <v>272</v>
+      </c>
+      <c r="F81">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A82" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="B82" t="s">
+        <v>123</v>
+      </c>
+      <c r="C82" t="s">
+        <v>273</v>
+      </c>
+      <c r="D82" t="s">
+        <v>274</v>
+      </c>
+      <c r="F82">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A83" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B83" t="s">
+        <v>127</v>
+      </c>
+      <c r="C83" t="s">
+        <v>275</v>
+      </c>
+      <c r="D83" t="s">
+        <v>276</v>
+      </c>
+      <c r="F83">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>9</v>
+      </c>
+      <c r="B84" t="s">
+        <v>122</v>
+      </c>
+      <c r="C84" t="s">
+        <v>277</v>
+      </c>
+      <c r="D84" t="s">
+        <v>278</v>
+      </c>
+      <c r="F84">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>21</v>
+      </c>
+      <c r="B85" t="s">
+        <v>122</v>
+      </c>
+      <c r="C85" t="s">
+        <v>279</v>
+      </c>
+      <c r="D85" t="s">
+        <v>280</v>
+      </c>
+      <c r="F85">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A86" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="B86" t="s">
+        <v>124</v>
+      </c>
+      <c r="C86" t="s">
+        <v>281</v>
+      </c>
+      <c r="D86" t="s">
+        <v>282</v>
+      </c>
+      <c r="F86">
+        <f t="shared" si="1"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A87" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B87" t="s">
+        <v>122</v>
+      </c>
+      <c r="C87" t="s">
+        <v>283</v>
+      </c>
+      <c r="D87" t="s">
+        <v>284</v>
+      </c>
+      <c r="F87">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>